<commit_message>
feat: add ehabibn-git.md profile
Commit do projeto dataset-gameshop de ehabibn-git.
</commit_message>
<xml_diff>
--- a/data/processed_data/Meganium_Sales_data.xlsx
+++ b/data/processed_data/Meganium_Sales_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\records\raw\curso prompt de vendas\project base\data\processed_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\dio.me\prompts-vendas\data\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF384361-7EE9-44FF-94D0-6781DB5A913D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E30CC2-3F7B-45FD-B578-A94D16D964DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20310" yWindow="-435" windowWidth="19260" windowHeight="10245" xr2:uid="{6AE332F9-81B0-4A6E-884F-846423EA80AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A0712B9-5B1D-4C87-9A49-2AA682D34034}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidate" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -879,15 +880,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -950,39 +950,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1034,7 +1034,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1145,13 +1145,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1160,6 +1153,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1224,43 +1224,63 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F4AE2D-9E03-435C-8CF9-67685E40A2EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7B9C3F-ABAB-40FD-B89C-AAE26F01F2C1}">
   <sheetPr>
-    <tabColor theme="9"/>
+    <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3948,8 +3968,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{C5F4AE2D-9E03-435C-8CF9-67685E40A2EE}"/>
+  <autoFilter ref="A1:N1" xr:uid="{8D7B9C3F-ABAB-40FD-B89C-AAE26F01F2C1}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>